<commit_message>
autocorrect values for algorithm
οι πιθανοι συνδυασμοι τροπου γραφης για καθε εντολη του αλγοριθμου
</commit_message>
<xml_diff>
--- a/AUTOCORRECT.xlsx
+++ b/AUTOCORRECT.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Diplomatiki\glossa_aepp_web_interpreter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CF5C067-F938-4D90-ADBC-77ADB34C4901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96046703-BAC0-4773-A0C9-A4DFB19FC438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15720" xr2:uid="{CCB591B9-2B09-45C9-9B3D-CA893BBB8B5A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CCB591B9-2B09-45C9-9B3D-CA893BBB8B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="314">
   <si>
     <t>Αλγόριθμος</t>
   </si>
@@ -446,27 +446,9 @@
     <t>ΑΡΧΗ_ΕΠΑΝΑΛΗΨΗΣ</t>
   </si>
   <si>
-    <t>ΜΕΧΡΙΣ_ΟΤΟΥ</t>
-  </si>
-  <si>
     <t>ΑΠΟΤΕΛΕΣΜΑΤΑ</t>
   </si>
   <si>
-    <r>
-      <t>ΤΕΛΟΣ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Lucida Console"/>
-        <family val="3"/>
-        <charset val="161"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
     <t>emfanise</t>
   </si>
   <si>
@@ -855,13 +837,166 @@
   </si>
   <si>
     <t>Επανάλαβε</t>
+  </si>
+  <si>
+    <t>ΌΛΑ ΚΕΦΑΛΑΙΑ και λαθος "Σ"</t>
+  </si>
+  <si>
+    <t>ΑΛΓΟΡΙΘΜΟς</t>
+  </si>
+  <si>
+    <t>ΑΛΛΙΩς_ΑΝ</t>
+  </si>
+  <si>
+    <t>ΑΛΛΙΩς</t>
+  </si>
+  <si>
+    <t>ΤΕΛΟς_ΕΠΑΝΑΛΗΨΗς</t>
+  </si>
+  <si>
+    <t>ΑΡΧΗ_ΕΠΑΝΑΛΗΨΗς</t>
+  </si>
+  <si>
+    <t>ΜΕΧΡΙς_ΟΤΟΥ</t>
+  </si>
+  <si>
+    <t>ΤΕΛΟς</t>
+  </si>
+  <si>
+    <t>αλλιωσ</t>
+  </si>
+  <si>
+    <t>Αλλιωσ</t>
+  </si>
+  <si>
+    <t>Αλλιώσ</t>
+  </si>
+  <si>
+    <t>ΤΕΛΟς_ΑΝ</t>
+  </si>
+  <si>
+    <t>τελοσ_αν</t>
+  </si>
+  <si>
+    <t>Τελοσ_αν</t>
+  </si>
+  <si>
+    <t>Τέλοσ_αν</t>
+  </si>
+  <si>
+    <t>τελοσ_επαναληψησ</t>
+  </si>
+  <si>
+    <t>τέλοσ_επανάληψησ</t>
+  </si>
+  <si>
+    <t>Τελοσ_επαναληψησ</t>
+  </si>
+  <si>
+    <t>αρχη_επαναληψησ</t>
+  </si>
+  <si>
+    <t>αρχή_επανάληψησ</t>
+  </si>
+  <si>
+    <t>Αρχη_επαναληψησ</t>
+  </si>
+  <si>
+    <t>τελοσ</t>
+  </si>
+  <si>
+    <t>τέλοσ</t>
+  </si>
+  <si>
+    <t>Τελοσ</t>
+  </si>
+  <si>
+    <t>ΤΕΛΟΣ</t>
+  </si>
+  <si>
+    <t>allivw_an</t>
+  </si>
+  <si>
+    <t>alli;vw_an</t>
+  </si>
+  <si>
+    <t>Allivw_an</t>
+  </si>
+  <si>
+    <t>Alli;vw_an</t>
+  </si>
+  <si>
+    <t>allivs</t>
+  </si>
+  <si>
+    <t>alli;vs</t>
+  </si>
+  <si>
+    <t>t;elos_an</t>
+  </si>
+  <si>
+    <t>Allivs</t>
+  </si>
+  <si>
+    <t>Telos_an</t>
+  </si>
+  <si>
+    <t>Alli;vs</t>
+  </si>
+  <si>
+    <t>T;elos_an</t>
+  </si>
+  <si>
+    <t>ALLIVS</t>
+  </si>
+  <si>
+    <t>telos_epanalhchs</t>
+  </si>
+  <si>
+    <t>arxh_epanalhchs</t>
+  </si>
+  <si>
+    <t>t;elos_epan;alhchs</t>
+  </si>
+  <si>
+    <t>arx;h_epan;alhchs</t>
+  </si>
+  <si>
+    <t>t;elos</t>
+  </si>
+  <si>
+    <t>Telos_epanalhchs</t>
+  </si>
+  <si>
+    <t>Arxh_epanalhchs</t>
+  </si>
+  <si>
+    <t>Telos</t>
+  </si>
+  <si>
+    <t>T;elos_epan;alhchs</t>
+  </si>
+  <si>
+    <t>Arx;h_epan;alhchs</t>
+  </si>
+  <si>
+    <t>T;elos</t>
+  </si>
+  <si>
+    <t>TELOS_EPANALHCHS</t>
+  </si>
+  <si>
+    <t>ARXH_EPANALHCHS</t>
+  </si>
+  <si>
+    <t>ALLIVW_AN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -894,22 +1029,22 @@
       <family val="3"/>
       <charset val="161"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1008,50 +1143,70 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1060,32 +1215,40 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -1094,123 +1257,57 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
@@ -1545,16 +1642,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{918D948B-F2B9-4D0F-8F55-03FA118DCD07}">
-  <dimension ref="A1:X21"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F14" sqref="F14"/>
+      <selection pane="topRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="39.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
@@ -1579,397 +1676,392 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="18" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="L2" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="M2" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="P2" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q2" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="S2" s="12" t="s">
+      <c r="S2" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="W2" s="12" t="s">
+      <c r="W2" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="19" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24" t="s">
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="S3" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="T3" s="24" t="s">
+      <c r="S3" s="11"/>
+      <c r="T3" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="U3" s="24" t="s">
+      <c r="U3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="V3" s="24" t="s">
+      <c r="V3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="W3" s="24" t="s">
+      <c r="W3" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="X3" s="15" t="s">
+      <c r="X3" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="24" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="24" t="s">
+      <c r="N4" s="11"/>
+      <c r="O4" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="T4" s="24" t="s">
+      <c r="T4" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="W4" s="24" t="s">
+      <c r="W4" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="X4" s="15" t="s">
+      <c r="X4" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="22" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="24" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="P5" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="24" t="s">
+      <c r="Q5" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="R5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="Q5" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="R5" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24"/>
-      <c r="X5" s="15"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="2"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="6"/>
+      <c r="B6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="K6" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="N6" s="16" t="s">
+      <c r="K6" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="N6" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="O6" s="16" t="s">
+      <c r="O6" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="Q6" s="16" t="s">
+      <c r="Q6" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="R6" s="16" t="s">
+      <c r="R6" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="S6" s="16" t="s">
+      <c r="S6" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="T6" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="V6" s="16" t="s">
+      <c r="T6" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="U6" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="V6" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="W6" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="W6" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="X6" s="15" t="s">
-        <v>134</v>
+      <c r="X6" s="3" t="s">
+        <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="12" t="s">
@@ -1979,351 +2071,351 @@
         <v>61</v>
       </c>
       <c r="E7" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="I7" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="J7" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>140</v>
-      </c>
       <c r="K7" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="N7" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="L7" s="12" t="s">
+      <c r="O7" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q7" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="R7" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="T7" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="U7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="V7" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="W7" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="W8" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="L9" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M9" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="N7" s="12" t="s">
-        <v>143</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="T7" s="12" t="s">
+      <c r="N9" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="O9" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="T9" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="U7" s="12" t="s">
+      <c r="U9" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="V7" s="12" t="s">
+      <c r="V9" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="W7" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="X7" s="13" t="s">
+      <c r="W9" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="U10" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="V10" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="W10" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="X10" s="2" t="s">
         <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>155</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q8" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="R8" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="S8" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="T8" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="U8" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="V8" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="W8" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="X8" s="13" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="19"/>
-      <c r="B9" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>170</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="M9" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="N9" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="O9" s="24" t="s">
-        <v>178</v>
-      </c>
-      <c r="P9" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q9" s="24" t="s">
-        <v>180</v>
-      </c>
-      <c r="R9" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="S9" s="24" t="s">
-        <v>182</v>
-      </c>
-      <c r="T9" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="U9" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="V9" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="W9" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="X9" s="13" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>199</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="P10" s="12" t="s">
-        <v>205</v>
-      </c>
-      <c r="Q10" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="R10" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="S10" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="T10" s="12" t="s">
-        <v>209</v>
-      </c>
-      <c r="U10" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="V10" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="W10" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="X10" s="13" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="23" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="H11" s="13" t="s">
         <v>215</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="I11" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="J11" s="13" t="s">
         <v>217</v>
       </c>
-      <c r="I11" s="25" t="s">
-        <v>218</v>
-      </c>
-      <c r="J11" s="25" t="s">
+      <c r="K11" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="L11" s="13" t="s">
         <v>219</v>
       </c>
-      <c r="K11" s="25" t="s">
+      <c r="M11" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="L11" s="25" t="s">
+      <c r="N11" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="M11" s="25" t="s">
+      <c r="O11" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="N11" s="25" t="s">
+      <c r="P11" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="O11" s="25" t="s">
+      <c r="Q11" s="13" t="s">
         <v>224</v>
       </c>
-      <c r="P11" s="25" t="s">
+      <c r="R11" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="Q11" s="25" t="s">
+      <c r="S11" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="R11" s="25" t="s">
+      <c r="T11" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="S11" s="25" t="s">
+      <c r="U11" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="T11" s="25" t="s">
+      <c r="V11" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="U11" s="26" t="s">
+      <c r="W11" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="V11" s="26" t="s">
+      <c r="X11" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="W11" s="26" t="s">
-        <v>232</v>
-      </c>
-      <c r="X11" s="27" t="s">
-        <v>233</v>
-      </c>
     </row>
-    <row r="12" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="12" t="s">
         <v>56</v>
       </c>
       <c r="C12" s="12" t="s">
@@ -2332,108 +2424,108 @@
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="H12" s="12" t="s">
-        <v>236</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="L12" s="12" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="R12" s="12"/>
       <c r="S12" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="T12" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="U12" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="T12" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="U12" s="12" t="s">
-        <v>242</v>
-      </c>
       <c r="V12" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="W12" s="12"/>
+      <c r="X12" s="20" t="s">
         <v>149</v>
-      </c>
-      <c r="W12" s="12"/>
-      <c r="X12" s="13" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="26" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="H13" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="G13" s="26" t="s">
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="L13" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26" t="s">
+      <c r="M13" s="13" t="s">
         <v>246</v>
       </c>
-      <c r="L13" s="26" t="s">
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="M13" s="26" t="s">
+      <c r="R13" s="13"/>
+      <c r="S13" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
-      <c r="Q13" s="26" t="s">
+      <c r="T13" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="R13" s="26"/>
-      <c r="S13" s="26" t="s">
+      <c r="U13" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="T13" s="26" t="s">
+      <c r="V13" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="U13" s="26" t="s">
+      <c r="W13" s="13"/>
+      <c r="X13" s="21" t="s">
         <v>252</v>
-      </c>
-      <c r="V13" s="26" t="s">
-        <v>253</v>
-      </c>
-      <c r="W13" s="26"/>
-      <c r="X13" s="27" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="12" t="s">
@@ -2447,246 +2539,398 @@
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+        <v>253</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>275</v>
+      </c>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
-      <c r="T14" s="12"/>
-      <c r="U14" s="12"/>
+      <c r="T14" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="U14" s="12" t="s">
+        <v>281</v>
+      </c>
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
-      <c r="X14" s="13"/>
+      <c r="X14" s="1" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="24" t="s">
-        <v>256</v>
-      </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="15"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>282</v>
+      </c>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="2" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="15"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11" t="s">
+        <v>280</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="V16" s="11"/>
+      <c r="W16" s="11"/>
+      <c r="X16" s="2" t="s">
+        <v>286</v>
+      </c>
     </row>
-    <row r="17" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="17"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>273</v>
+      </c>
+      <c r="M17" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="2"/>
     </row>
-    <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="U18" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C19" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="12"/>
-      <c r="S18" s="12"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="13"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="15"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="U19" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11" t="s">
+        <v>302</v>
+      </c>
+      <c r="U20" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+      <c r="X20" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="15"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="L21" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>296</v>
+      </c>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="U21" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+      <c r="X21" s="2" t="s">
+        <v>307</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="8" t="s">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="16"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
-      <c r="S21" s="16"/>
-      <c r="T21" s="16"/>
-      <c r="U21" s="16"/>
-      <c r="V21" s="16"/>
-      <c r="W21" s="16"/>
-      <c r="X21" s="17"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="L22" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="U22" s="11" t="s">
+        <v>309</v>
+      </c>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+      <c r="X22" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="U23" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A19:A23"/>
     <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>